<commit_message>
v 0.6 - Silicon - Fiber termination
</commit_message>
<xml_diff>
--- a/Arbeitsplan_fos4Acc_allV0.4.xlsx
+++ b/Arbeitsplan_fos4Acc_allV0.4.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ubuntuserver\Users\Flehr\Desktop\Python\FBGAcc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="270" yWindow="600" windowWidth="28215" windowHeight="11955" activeTab="1"/>
+    <workbookView xWindow="270" yWindow="600" windowWidth="20730" windowHeight="11760" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="acc_Rahmen" sheetId="1" r:id="rId1"/>
@@ -12,13 +17,15 @@
     <sheet name="acc_Konfektionierung" sheetId="3" r:id="rId3"/>
     <sheet name="acc_QC" sheetId="5" r:id="rId4"/>
     <sheet name="Tabelle1" sheetId="6" r:id="rId5"/>
+    <sheet name="acc_Silikon" sheetId="7" r:id="rId6"/>
+    <sheet name="acc_Terminierung" sheetId="8" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="83">
   <si>
     <t>Referenz</t>
   </si>
@@ -80,9 +87,6 @@
     <t>Faser in Rahmen und Balken positionieren</t>
   </si>
   <si>
-    <t>Faserspitze mit FBG durch obere, große Öffnung des Rahmen und Balken schieben, so dass das FBG grob zwischen Balken und Rahmen (links) positioniert ist. Faser beidseitig des Rahmens mit den Klemmen fixieren. Darauf achten, das die Faser entspannt ist!  "Weiter"</t>
-  </si>
-  <si>
     <t>peak, temp, spectrum,  fwhm, asymm</t>
   </si>
   <si>
@@ -95,9 +99,6 @@
     <t>Justage FBG</t>
   </si>
   <si>
-    <t>Das FBG mittels Laser/Fiber Checker mittig zwischen Blaken und Rahmen positionieren. "Weiter"</t>
-  </si>
-  <si>
     <t>Vorspannung genau</t>
   </si>
   <si>
@@ -122,9 +123,6 @@
     <t>Bügeleisen mit 160°C mittig auf den Sensor stellen und ca. 8 min aushärten lassen.   "Weiter"</t>
   </si>
   <si>
-    <t>cooling</t>
-  </si>
-  <si>
     <t>Abkühlen lassen</t>
   </si>
   <si>
@@ -194,9 +192,6 @@
     <t xml:space="preserve">Sensor auf die Seite (Faserabführung) stellen und mit "Weiter" bestätigen </t>
   </si>
   <si>
-    <t>Faser an die Faser-Kupplung des Spektrometers anschließen. Faser im Bereich des FBG mit Alkohol reinigen. Geben Sie die Sensor- und FBG-Identifikationskennung ein. "Weiter"</t>
-  </si>
-  <si>
     <t>- 900µm Buffer (gelber Schlauch) auf 35cm ablängen</t>
   </si>
   <si>
@@ -218,7 +213,67 @@
     <t>- Silikon durch Rahmenöffnung einfüllen (0,5ml), zuerst Loch im Balken füllen, dann Klebetropfen bilden und in Rahmenöffnung austreten lassen, mindestens 24h aushärten lassen</t>
   </si>
   <si>
-    <t>ids, fbg</t>
+    <t>Wellenlänge einstellen</t>
+  </si>
+  <si>
+    <t>Sensor mittels Schrauben auf die geforderte Wellenlänge einstellen</t>
+  </si>
+  <si>
+    <t>peak</t>
+  </si>
+  <si>
+    <t>Silikon einfüllen</t>
+  </si>
+  <si>
+    <t>Wellenlänge kontrollieren</t>
+  </si>
+  <si>
+    <t>Kontrollieren ob sich die Wellenlänge im entsprechenden Bereich befindet, evtl. nachjustieren</t>
+  </si>
+  <si>
+    <t>Fertig</t>
+  </si>
+  <si>
+    <t>Sensor zur Aushärtung des Silikons abstellen</t>
+  </si>
+  <si>
+    <t>Silikon mit Spritze (Spezialkanüle) zuerst an Balken auftragen, dann durch Rahmen bis sich Klebetropfen bildet. Immer definierte Menge an Silikon verwenden =&gt; 0,5 ml. Mindestens 24 h aushärten lassen.</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>ids,  fbg</t>
+  </si>
+  <si>
+    <t>ids, date</t>
+  </si>
+  <si>
+    <t>ids</t>
+  </si>
+  <si>
+    <t>Faserschleife</t>
+  </si>
+  <si>
+    <t>Faser kürzen</t>
+  </si>
+  <si>
+    <t>Faserende zur engen Schleife ziehen bis bis Wert "Rückkopplung" minimal wird</t>
+  </si>
+  <si>
+    <t>Faser innerhalb des Rahmens mittels Nagelschere abschneiden, kontrollieren ob "Rückkopplung" mindestens den Zielwer erreicht, ggf. weiter kürzen</t>
+  </si>
+  <si>
+    <t>Sensor abstecken und zur Verklebung des Faserendes abstellen, Verklebung: Bohrung Faserende mit UHU schnellfest auffüllen</t>
+  </si>
+  <si>
+    <t>Das Fasergitter mittels Laser/Fiber Checker mittig zwischen Blaken und Rahmen positionieren. "Weiter"</t>
+  </si>
+  <si>
+    <t>Faserspitze durch obere, große Öffnung des Rahmen und Balken schieben, so dass das Fasergitter grob zwischen Balken und Rahmen (links) positioniert ist. Faser beidseitig des Rahmens mit den Klemmen fixieren. Darauf achten, das die Faser entspannt ist!  "Weiter"</t>
+  </si>
+  <si>
+    <t>Faser an die Faser-Kupplung des Spektrometers anschließen. Faser im Bereich des Fasergitters mit Alkohol reinigen. Geben Sie die Sensor- und Faser-Identifikationskennung ein. "Weiter"</t>
   </si>
 </sst>
 </file>
@@ -695,7 +750,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -734,7 +789,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -789,7 +844,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -827,9 +882,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -867,9 +922,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -904,7 +959,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -939,7 +994,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1177,8 +1232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J84"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A7" zoomScale="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView view="pageLayout" topLeftCell="C1" zoomScale="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1268,13 +1323,15 @@
         <v>1</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+      <c r="I3" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="J3" s="25" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1294,12 +1351,12 @@
         <v>1</v>
       </c>
       <c r="F4" s="32" t="s">
-        <v>20</v>
+        <v>81</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J4" s="2"/>
     </row>
@@ -1314,13 +1371,13 @@
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="25">
+        <v>1</v>
+      </c>
+      <c r="F5" s="32" t="s">
         <v>22</v>
-      </c>
-      <c r="E5" s="25">
-        <v>1</v>
-      </c>
-      <c r="F5" s="32" t="s">
-        <v>23</v>
       </c>
       <c r="G5" s="2">
         <v>1</v>
@@ -1342,13 +1399,13 @@
         <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" s="2">
         <v>1</v>
       </c>
       <c r="F6" s="32" t="s">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -1366,20 +1423,20 @@
         <v>6</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E7" s="25">
         <v>1</v>
       </c>
       <c r="F7" s="32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G7" s="2">
         <v>2</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>10</v>
@@ -1396,18 +1453,18 @@
         <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E8" s="2">
         <v>1</v>
       </c>
       <c r="F8" s="32" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="1" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1421,19 +1478,17 @@
         <v>8</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E9" s="2">
         <v>1</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10" s="1" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1447,11 +1502,11 @@
         <v>9</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -1949,7 +2004,7 @@
   <dimension ref="A4:D44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1963,13 +2018,13 @@
         <v>14</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1977,13 +2032,13 @@
         <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C5" s="25">
         <v>1</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -1991,7 +2046,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -2003,7 +2058,7 @@
         <v>17</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C7" s="25">
         <v>1</v>
@@ -2013,37 +2068,37 @@
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="D10" s="35" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="D11" s="36" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="D12" s="36" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="D13" s="36" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D14" s="37" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D15" s="35" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D16" s="37" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.25">
@@ -2142,7 +2197,7 @@
   <dimension ref="A3:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection sqref="A1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2190,13 +2245,13 @@
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E4" s="2">
         <v>1</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -2213,18 +2268,18 @@
         <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E5" s="25">
         <v>1</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -2238,18 +2293,18 @@
         <v>3</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E6" s="2">
         <v>1</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -2263,18 +2318,18 @@
         <v>4</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E7" s="2">
         <v>2</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -2303,13 +2358,13 @@
         <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E1" s="25">
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -2326,13 +2381,13 @@
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -2349,17 +2404,379 @@
         <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E3" s="25">
         <v>1</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="38.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J2" s="25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="12">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="25">
+        <v>1</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="2">
+        <v>3</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" s="2">
+        <v>3</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+      <c r="F6" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J9" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="37.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J2" s="25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="12">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" s="25">
+        <v>1</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="G3" s="2">
+        <v>4</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" s="2">
+        <v>4</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="25"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>